<commit_message>
mejor gestion de reglas de formato
</commit_message>
<xml_diff>
--- a/templates/template.xlsx
+++ b/templates/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ernesto Palacios\GIT\pandas-to-excel-automation\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE73D08-7C30-41C9-AF28-0691A2EC7845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C6DA868-DF54-493D-AA12-8AC06C3E7658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28560" windowHeight="14775" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7889" uniqueCount="1027">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7889" uniqueCount="1028">
   <si>
     <t>CUENTAS</t>
   </si>
@@ -3629,6 +3629,9 @@
   <si>
     <t>Cuzuntza Alto, daño informado por el Sr. Alejandro Dávila previa
 revisión en la estructura. 28303 se cambia tirafusible quemado de 6 Amp tipo T, CAUSA: Vegetación, CARGA: 30KVA.</t>
+  </si>
+  <si>
+    <t>Texto</t>
   </si>
 </sst>
 </file>
@@ -3845,7 +3848,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="65">
+  <dxfs count="46">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3904,8 +3907,11 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF000000"/>
       </font>
     </dxf>
@@ -3916,35 +3922,8 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.3498947111423078"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
+        <b/>
+        <i val="0"/>
         <color rgb="FF000000"/>
       </font>
     </dxf>
@@ -3969,6 +3948,123 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF77933C"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFFC000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4050,19 +4146,17 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF000000"/>
       </font>
     </dxf>
     <dxf>
       <font>
         <color theme="3"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
       </font>
     </dxf>
     <dxf>
@@ -4091,308 +4185,8 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF000000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b/>
         <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1" tint="0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF77933C"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFFC000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.3498947111423078"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1" tint="0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF77933C"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFFC000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.3498947111423078"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF000000"/>
       </font>
     </dxf>
@@ -5230,8 +5024,8 @@
   <dimension ref="A1:W515"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M1" sqref="M1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5547,7 +5341,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="105" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -5555,7 +5349,7 @@
         <v>79</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>97</v>
+        <v>1027</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>7</v>
@@ -34944,62 +34738,59 @@
   </sheetData>
   <autoFilter ref="A1:W293" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <conditionalFormatting sqref="A1:A1048576 L1:L1048576">
-    <cfRule type="containsText" dxfId="15" priority="9" operator="containsText" text="domingo">
+    <cfRule type="containsText" dxfId="29" priority="9" operator="containsText" text="sábado">
+      <formula>NOT(ISERROR(SEARCH("sábado",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="28" priority="10" operator="containsText" text="domingo">
       <formula>NOT(ISERROR(SEARCH("domingo",A1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="7" operator="containsText" text="sábado">
-      <formula>NOT(ISERROR(SEARCH("sábado",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:X1048576">
-    <cfRule type="expression" dxfId="13" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="16">
       <formula>$A1=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="17">
       <formula>$B1="se_labora"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:C1048576">
-    <cfRule type="cellIs" dxfId="11" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="5" operator="equal">
+      <formula>"REDES"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="7" operator="equal">
+      <formula>"ALUMBRADO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="18" operator="equal">
       <formula>"MEDIDORES"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="15" operator="equal">
-      <formula>"se_labora"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="19" operator="equal">
       <formula>"informativa"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="16" operator="equal">
-      <formula>"ALUMBRADO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="4" stopIfTrue="1" operator="equal">
-      <formula>"REDES"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="expression" dxfId="6" priority="19">
+    <cfRule type="expression" dxfId="22" priority="1">
       <formula>$S1="Si"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="NO PROG">
+    <cfRule type="containsText" dxfId="21" priority="2" operator="containsText" text="NO PROG">
       <formula>NOT(ISERROR(SEARCH("NO PROG",D1)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="4" operator="equal">
       <formula>"PROG"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="cellIs" dxfId="3" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="11" operator="equal">
       <formula>"EXPANSION"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="12" operator="equal">
       <formula>"PREDICTIVO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
       <formula>"PREVENTIVO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="14" operator="equal">
       <formula>"CORRECTIVO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -35007,7 +34798,7 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="6">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Revisar" error="El valor introducido no se reconoce" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
             <xm:f>LISTAS!$B$3:$B$16</xm:f>

</xml_diff>